<commit_message>
Changes to Task3 with the maxRows now a lot less since only 116 violationTypes occur.
</commit_message>
<xml_diff>
--- a/ViolationTypes.xlsx
+++ b/ViolationTypes.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1105,6 +1105,1012 @@
         <v>5515</v>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>F049</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t># 50. Impoundment of unsanitary equipment or food</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>5928</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>F050</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t># 51. Permit Suspension</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>2955</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>F051</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t># 49. Samples Collected</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>F052</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t># 01b. Food safety certification</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>18359</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>F053</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t># 21a. Hot Water Available</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>4218</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>F054</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t># 52. Multiple Major Critical Violations / Increased Risk to Public Health</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>F055</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t># 01a. Demonstration of knowledge</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>F056</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t># 10. Proper cooking time &amp; temperatures</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>F057</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t># 18. Compliance with variance, specialized process, &amp; HACCP Plan</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>F058</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t># 19. Consumer advisory provided for raw or undercooked foods</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>MF07</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t># 07. Adequate handwashing facilities supplied &amp; accessible</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>MF42</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t># 42. Garbage and refuse properly disposed; facilities maintained</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>SF15</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>No Health Code Violations Observed At The Time Of Inspection</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>SS33</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Garbage / rubbish receptacles not maintained clean and sanitary</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>W001</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Proper hot and cold holding temperatures</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>W002</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Food in good condition, safe and unadultered</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>W003</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Food storage separated and protected</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>W004</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Food storage space</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>W005</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Food elevated</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>W006</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Food packaging protected</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>W008</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Rodent</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>W009</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Cockroaches</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>W011</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Storage of materials 18 inches above the floor.</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>W012</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Fly Breeding Material</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>W014</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Fly Breeding</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>W016</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Building rodent proof</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>W017</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Hot and cold water available</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>W018</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Waste water or sewage properly disposed or not discharged on the ground.</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>W019</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Plumbing approved and maintained in good repair.</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>W020</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Wall(s) maintained clean</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>W021</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Wall(s) maintained in good repair</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>W022</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Wall(s) constructed of approved material</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>W023</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Floor maintained clean</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>W024</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Floor maintained in good repair</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>W025</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Ceiling maintained clean</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>W026</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Ceiling maintained in good repair</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>W027</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Ceiling constructed of smooth, durable, and non-absorbent material</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>W028</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Toilet in good repair</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>W029</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Toilet maintained clean / sanitary</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>W030</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Hand sink in good repair</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>W031</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Hand sink maintained clean / sanitary</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>W032</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Toilet room floor / walls / ceiling in good repair</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>W033</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Toilet room floor / walls / ceiling clean</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>W034</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Toilet room with toilet paper / soap / towels / trash receptacle</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>W035</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Toilet room well ventilated</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>W036</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Toilet room well lighted</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>W037</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Toilet available</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>W038</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Hand sink available</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>W039</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Proper storage or use of hazardous materials</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>W040</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Compliance with shellfish tag requirements</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>W041</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Premises maintained clean and sanitary</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>W042</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Garbage / Rubbish receptacles approved type</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>W043</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Garbage / Rubbish receptacles maintained in good repair</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>W044</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Garbage / Rubbish receptacles maintained clean and sanitary</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>W045</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>No unapproved sleeping accomodations</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>W046</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Live animals</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>W047</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Thermometer: available, maintained in good repair</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>W048</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Permits Available</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>W049</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Food from an approved source</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>W050</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Food properly labeled</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>W051</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Walls, Floors, Ceilings: approved, maintained clean and in good repair</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>W052</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Equipment, Shelving, Cabinets: approved, maintained clean and in good repair</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>W053</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Permit Suspension</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>WP13</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t># 13. Disease Transmission - Carrier / Lesion / Rash</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>WP15</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t># 15. Tobacco / Eating / Drinking / Habits / Behaviors</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>WP16</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t># 16. Hair Restraints / Outer Garments / Nails / Rings</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>WP18</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t># 18. Personal Hygiene</t>
+        </is>
+      </c>
+      <c r="C117" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118"/>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Task 3 added with total sum of the count.
</commit_message>
<xml_diff>
--- a/ViolationTypes.xlsx
+++ b/ViolationTypes.xlsx
@@ -2110,7 +2110,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118"/>
+    <row r="118">
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Total Sum</t>
+        </is>
+      </c>
+      <c r="C118" t="n">
+        <v>906014</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes to task 2 (now working as intended) and task4 part 2.
</commit_message>
<xml_diff>
--- a/ViolationTypes.xlsx
+++ b/ViolationTypes.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +49,9 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -354,17 +358,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Code</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Count</t>
         </is>

</xml_diff>